<commit_message>
Filter2: BOM - wip
</commit_message>
<xml_diff>
--- a/modules/Filter2/Filter2-BOM.xlsx
+++ b/modules/Filter2/Filter2-BOM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\Filter2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{786589E1-1BDD-4F19-892A-0E57CE1F60F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107DE71E-5CE9-42FE-B7FE-82E8A4D1B436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7110" yWindow="1530" windowWidth="18540" windowHeight="12495"/>
+    <workbookView xWindow="9165" yWindow="1545" windowWidth="18540" windowHeight="12495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Filter2-BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -367,9 +380,6 @@
     <t>J109</t>
   </si>
   <si>
-    <t>Conn_Eurorack_16</t>
-  </si>
-  <si>
     <t>Eurorack 10-pin board power connector</t>
   </si>
   <si>
@@ -632,12 +642,15 @@
   </si>
   <si>
     <t>Need</t>
+  </si>
+  <si>
+    <t>Conn_Eurorack_10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1483,11 +1496,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1504,13 +1517,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -1568,9 +1581,12 @@
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
       <c r="E2">
         <f>MAX(0,B2-(C2+D2))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="s">
         <v>19</v>
@@ -1607,9 +1623,12 @@
       <c r="B3">
         <v>4</v>
       </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
       <c r="E3">
         <f t="shared" ref="E3:E28" si="0">MAX(0,B3-(C3+D3))</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F3" t="s">
         <v>29</v>
@@ -1718,9 +1737,12 @@
       <c r="B6">
         <v>2</v>
       </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F6" t="s">
         <v>53</v>
@@ -1769,9 +1791,12 @@
       <c r="B7">
         <v>6</v>
       </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F7" t="s">
         <v>65</v>
@@ -1808,9 +1833,12 @@
       <c r="B8">
         <v>2</v>
       </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F8" t="s">
         <v>72</v>
@@ -1826,9 +1854,12 @@
       <c r="B9">
         <v>1</v>
       </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" t="s">
         <v>75</v>
@@ -1934,9 +1965,12 @@
       <c r="B11">
         <v>1</v>
       </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" t="s">
         <v>99</v>
@@ -1970,9 +2004,12 @@
       <c r="B12">
         <v>1</v>
       </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" t="s">
         <v>105</v>
@@ -2006,9 +2043,12 @@
       <c r="B13">
         <v>1</v>
       </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" t="s">
         <v>110</v>
@@ -2042,9 +2082,12 @@
       <c r="B14">
         <v>1</v>
       </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" t="s">
         <v>113</v>
@@ -2078,21 +2121,24 @@
       <c r="B15">
         <v>1</v>
       </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" t="s">
+        <v>203</v>
+      </c>
+      <c r="I15" t="s">
         <v>115</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>116</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>117</v>
-      </c>
-      <c r="K15" t="s">
-        <v>118</v>
       </c>
       <c r="L15">
         <v>61201021621</v>
@@ -2101,10 +2147,10 @@
         <v>34</v>
       </c>
       <c r="N15" t="s">
+        <v>118</v>
+      </c>
+      <c r="O15" t="s">
         <v>119</v>
-      </c>
-      <c r="O15" t="s">
-        <v>120</v>
       </c>
       <c r="P15" t="s">
         <v>22</v>
@@ -2115,7 +2161,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -2125,36 +2171,36 @@
         <v>4</v>
       </c>
       <c r="F16" t="s">
+        <v>121</v>
+      </c>
+      <c r="G16" t="s">
         <v>122</v>
       </c>
-      <c r="G16" t="s">
+      <c r="I16" t="s">
         <v>123</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>124</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>125</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>126</v>
-      </c>
-      <c r="L16" t="s">
-        <v>127</v>
       </c>
       <c r="M16" t="s">
         <v>34</v>
       </c>
       <c r="N16" t="s">
+        <v>127</v>
+      </c>
+      <c r="O16" t="s">
         <v>128</v>
-      </c>
-      <c r="O16" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -2164,36 +2210,36 @@
         <v>4</v>
       </c>
       <c r="F17" t="s">
+        <v>130</v>
+      </c>
+      <c r="G17" t="s">
+        <v>122</v>
+      </c>
+      <c r="I17" t="s">
+        <v>123</v>
+      </c>
+      <c r="J17" t="s">
+        <v>124</v>
+      </c>
+      <c r="K17" t="s">
+        <v>125</v>
+      </c>
+      <c r="L17" t="s">
         <v>131</v>
-      </c>
-      <c r="G17" t="s">
-        <v>123</v>
-      </c>
-      <c r="I17" t="s">
-        <v>124</v>
-      </c>
-      <c r="J17" t="s">
-        <v>125</v>
-      </c>
-      <c r="K17" t="s">
-        <v>126</v>
-      </c>
-      <c r="L17" t="s">
-        <v>132</v>
       </c>
       <c r="M17" t="s">
         <v>34</v>
       </c>
       <c r="N17" t="s">
+        <v>132</v>
+      </c>
+      <c r="O17" t="s">
         <v>133</v>
-      </c>
-      <c r="O17" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B18">
         <v>8</v>
@@ -2203,36 +2249,36 @@
         <v>8</v>
       </c>
       <c r="F18" t="s">
+        <v>135</v>
+      </c>
+      <c r="G18" t="s">
+        <v>122</v>
+      </c>
+      <c r="I18" t="s">
+        <v>123</v>
+      </c>
+      <c r="J18" t="s">
+        <v>124</v>
+      </c>
+      <c r="K18" t="s">
+        <v>125</v>
+      </c>
+      <c r="L18" t="s">
         <v>136</v>
-      </c>
-      <c r="G18" t="s">
-        <v>123</v>
-      </c>
-      <c r="I18" t="s">
-        <v>124</v>
-      </c>
-      <c r="J18" t="s">
-        <v>125</v>
-      </c>
-      <c r="K18" t="s">
-        <v>126</v>
-      </c>
-      <c r="L18" t="s">
-        <v>137</v>
       </c>
       <c r="M18" t="s">
         <v>34</v>
       </c>
       <c r="N18" t="s">
+        <v>137</v>
+      </c>
+      <c r="O18" t="s">
         <v>138</v>
-      </c>
-      <c r="O18" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -2242,36 +2288,36 @@
         <v>4</v>
       </c>
       <c r="F19" t="s">
+        <v>140</v>
+      </c>
+      <c r="G19" t="s">
+        <v>122</v>
+      </c>
+      <c r="I19" t="s">
+        <v>123</v>
+      </c>
+      <c r="J19" t="s">
+        <v>124</v>
+      </c>
+      <c r="K19" t="s">
+        <v>125</v>
+      </c>
+      <c r="L19" t="s">
         <v>141</v>
-      </c>
-      <c r="G19" t="s">
-        <v>123</v>
-      </c>
-      <c r="I19" t="s">
-        <v>124</v>
-      </c>
-      <c r="J19" t="s">
-        <v>125</v>
-      </c>
-      <c r="K19" t="s">
-        <v>126</v>
-      </c>
-      <c r="L19" t="s">
-        <v>142</v>
       </c>
       <c r="M19" t="s">
         <v>34</v>
       </c>
       <c r="N19" t="s">
+        <v>142</v>
+      </c>
+      <c r="O19" t="s">
         <v>143</v>
-      </c>
-      <c r="O19" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -2281,36 +2327,36 @@
         <v>2</v>
       </c>
       <c r="F20" t="s">
+        <v>145</v>
+      </c>
+      <c r="G20" t="s">
+        <v>122</v>
+      </c>
+      <c r="I20" t="s">
+        <v>123</v>
+      </c>
+      <c r="J20" t="s">
+        <v>124</v>
+      </c>
+      <c r="K20" t="s">
+        <v>125</v>
+      </c>
+      <c r="L20" t="s">
         <v>146</v>
-      </c>
-      <c r="G20" t="s">
-        <v>123</v>
-      </c>
-      <c r="I20" t="s">
-        <v>124</v>
-      </c>
-      <c r="J20" t="s">
-        <v>125</v>
-      </c>
-      <c r="K20" t="s">
-        <v>126</v>
-      </c>
-      <c r="L20" t="s">
-        <v>147</v>
       </c>
       <c r="M20" t="s">
         <v>34</v>
       </c>
       <c r="N20" t="s">
+        <v>147</v>
+      </c>
+      <c r="O20" t="s">
         <v>148</v>
-      </c>
-      <c r="O20" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -2320,36 +2366,36 @@
         <v>4</v>
       </c>
       <c r="F21" t="s">
+        <v>150</v>
+      </c>
+      <c r="G21" t="s">
+        <v>122</v>
+      </c>
+      <c r="I21" t="s">
+        <v>123</v>
+      </c>
+      <c r="J21" t="s">
+        <v>124</v>
+      </c>
+      <c r="K21" t="s">
+        <v>125</v>
+      </c>
+      <c r="L21" t="s">
         <v>151</v>
-      </c>
-      <c r="G21" t="s">
-        <v>123</v>
-      </c>
-      <c r="I21" t="s">
-        <v>124</v>
-      </c>
-      <c r="J21" t="s">
-        <v>125</v>
-      </c>
-      <c r="K21" t="s">
-        <v>126</v>
-      </c>
-      <c r="L21" t="s">
-        <v>152</v>
       </c>
       <c r="M21" t="s">
         <v>34</v>
       </c>
       <c r="N21" t="s">
+        <v>152</v>
+      </c>
+      <c r="O21" t="s">
         <v>153</v>
-      </c>
-      <c r="O21" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B22">
         <v>4</v>
@@ -2359,36 +2405,36 @@
         <v>4</v>
       </c>
       <c r="F22" t="s">
+        <v>155</v>
+      </c>
+      <c r="G22" t="s">
+        <v>122</v>
+      </c>
+      <c r="I22" t="s">
+        <v>123</v>
+      </c>
+      <c r="J22" t="s">
+        <v>124</v>
+      </c>
+      <c r="K22" t="s">
+        <v>125</v>
+      </c>
+      <c r="L22" t="s">
         <v>156</v>
-      </c>
-      <c r="G22" t="s">
-        <v>123</v>
-      </c>
-      <c r="I22" t="s">
-        <v>124</v>
-      </c>
-      <c r="J22" t="s">
-        <v>125</v>
-      </c>
-      <c r="K22" t="s">
-        <v>126</v>
-      </c>
-      <c r="L22" t="s">
-        <v>157</v>
       </c>
       <c r="M22" t="s">
         <v>34</v>
       </c>
       <c r="N22" t="s">
+        <v>157</v>
+      </c>
+      <c r="O22" t="s">
         <v>158</v>
-      </c>
-      <c r="O22" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -2398,39 +2444,39 @@
         <v>2</v>
       </c>
       <c r="F23" t="s">
+        <v>160</v>
+      </c>
+      <c r="G23" t="s">
         <v>161</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>162</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
+        <v>123</v>
+      </c>
+      <c r="J23" t="s">
         <v>163</v>
       </c>
-      <c r="I23" t="s">
-        <v>124</v>
-      </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
+        <v>125</v>
+      </c>
+      <c r="L23" t="s">
         <v>164</v>
-      </c>
-      <c r="K23" t="s">
-        <v>126</v>
-      </c>
-      <c r="L23" t="s">
-        <v>165</v>
       </c>
       <c r="M23" t="s">
         <v>34</v>
       </c>
       <c r="N23" t="s">
+        <v>165</v>
+      </c>
+      <c r="O23" t="s">
         <v>166</v>
-      </c>
-      <c r="O23" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -2440,36 +2486,36 @@
         <v>2</v>
       </c>
       <c r="F24" t="s">
+        <v>168</v>
+      </c>
+      <c r="G24" t="s">
         <v>169</v>
       </c>
-      <c r="G24" t="s">
+      <c r="I24" t="s">
         <v>170</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>171</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>172</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>173</v>
-      </c>
-      <c r="L24" t="s">
-        <v>174</v>
       </c>
       <c r="M24" t="s">
         <v>22</v>
       </c>
       <c r="N24" t="s">
+        <v>174</v>
+      </c>
+      <c r="O24" t="s">
         <v>175</v>
-      </c>
-      <c r="O24" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -2479,36 +2525,36 @@
         <v>2</v>
       </c>
       <c r="F25" t="s">
+        <v>168</v>
+      </c>
+      <c r="G25" t="s">
         <v>169</v>
       </c>
-      <c r="G25" t="s">
-        <v>170</v>
-      </c>
       <c r="I25" t="s">
+        <v>177</v>
+      </c>
+      <c r="J25" t="s">
         <v>178</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
+        <v>172</v>
+      </c>
+      <c r="L25" t="s">
         <v>179</v>
-      </c>
-      <c r="K25" t="s">
-        <v>173</v>
-      </c>
-      <c r="L25" t="s">
-        <v>180</v>
       </c>
       <c r="M25" t="s">
         <v>22</v>
       </c>
       <c r="N25" t="s">
+        <v>174</v>
+      </c>
+      <c r="O25" t="s">
         <v>175</v>
-      </c>
-      <c r="O25" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -2518,36 +2564,36 @@
         <v>2</v>
       </c>
       <c r="F26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G26" t="s">
+        <v>169</v>
+      </c>
+      <c r="I26" t="s">
         <v>170</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>171</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>172</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>173</v>
-      </c>
-      <c r="L26" t="s">
-        <v>174</v>
       </c>
       <c r="M26" t="s">
         <v>22</v>
       </c>
       <c r="N26" t="s">
+        <v>174</v>
+      </c>
+      <c r="O26" t="s">
         <v>175</v>
-      </c>
-      <c r="O26" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -2557,42 +2603,42 @@
         <v>2</v>
       </c>
       <c r="F27" t="s">
+        <v>182</v>
+      </c>
+      <c r="I27" t="s">
         <v>183</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>184</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>185</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>186</v>
-      </c>
-      <c r="L27" t="s">
-        <v>187</v>
       </c>
       <c r="M27" t="s">
         <v>34</v>
       </c>
       <c r="N27" t="s">
+        <v>187</v>
+      </c>
+      <c r="O27" t="s">
         <v>188</v>
       </c>
-      <c r="O27" t="s">
+      <c r="P27" t="s">
         <v>189</v>
       </c>
-      <c r="P27" t="s">
+      <c r="Q27" t="s">
         <v>190</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="R27" t="s">
         <v>191</v>
-      </c>
-      <c r="R27" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -2602,28 +2648,28 @@
         <v>3</v>
       </c>
       <c r="F28" t="s">
+        <v>193</v>
+      </c>
+      <c r="I28" t="s">
         <v>194</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>195</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>196</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>197</v>
-      </c>
-      <c r="L28" t="s">
-        <v>198</v>
       </c>
       <c r="M28" t="s">
         <v>34</v>
       </c>
       <c r="N28" t="s">
+        <v>198</v>
+      </c>
+      <c r="O28" t="s">
         <v>199</v>
-      </c>
-      <c r="O28" t="s">
-        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>